<commit_message>
Move files and upload points
</commit_message>
<xml_diff>
--- a/Баллы 2025.xlsx
+++ b/Баллы 2025.xlsx
@@ -544,13 +544,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -622,6 +615,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -907,7 +907,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H16" sqref="H16"/>
+      <selection pane="topRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,8 +1059,12 @@
       <c r="C2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="D2" s="16">
+        <v>5</v>
+      </c>
+      <c r="E2" s="16">
+        <v>1</v>
+      </c>
       <c r="F2" s="16"/>
       <c r="G2" s="41"/>
       <c r="H2" s="38"/>
@@ -1084,7 +1088,7 @@
       <c r="Z2" s="17"/>
       <c r="AA2" s="12">
         <f t="shared" ref="AA2:AA11" si="0">SUM(C2:Z2)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AB2" s="18" t="str">
         <f t="shared" ref="AB2:AB11" si="1">IF(AA2&gt;=87,"отл",IF(AA2&gt;=73,"хорошо",IF(AA2&gt;=50,"удовл","Не удовл")))</f>
@@ -1656,7 +1660,7 @@
       <c r="L31" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="PQpqF2MK2ePNiXt8AvJ1uqtcXibZc2BrIfP6KRRMnBec5hoUQYshEh3sFIPYG+5brtBqx/xMl/MkN0TxO4eUMA==" saltValue="USmwV9KvNIQtH7n4E13N9Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="guTWOc3b1qN6dQq4E0M+bvAbOy96sJx39mVbiw2H6NVXotuJ4mJWN5SV3RqIKvxGaiMgZaRklokLzVhTmVk9uw==" saltValue="wFCknY9Dyx0xFljTiw45ig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
     <mergeCell ref="V12:X12"/>
     <mergeCell ref="Y12:Z12"/>
@@ -1677,49 +1681,49 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A11">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB11">
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Не">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Не">
       <formula>NOT(ISERROR(SEARCH("Не",AB2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="отл">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="отл">
       <formula>NOT(ISERROR(SEARCH("отл",AB2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="хорошо">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="хорошо">
       <formula>NOT(ISERROR(SEARCH("хорошо",AB2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="удовл">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="удовл">
       <formula>NOT(ISERROR(SEARCH("удовл",AB2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AC11">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="E">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="E">
       <formula>NOT(ISERROR(SEARCH("E",AC2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AC2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="C-">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="C-">
       <formula>NOT(ISERROR(SEARCH("C-",AC2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="A">
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH("A",AC2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="B+">
+    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="B+">
       <formula>NOT(ISERROR(SEARCH("B+",AC2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="14" operator="containsText" text="B">
+    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH("B",AC2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="15" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="1" priority="15" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",AC2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AD11">
-    <cfRule type="notContainsText" dxfId="1" priority="16" operator="notContains" text="не">
+    <cfRule type="notContainsText" dxfId="0" priority="16" operator="notContains" text="не">
       <formula>ISERROR(SEARCH("не",AD2))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>